<commit_message>
divided invalid and valid login and registration in multiples tests
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/data.xlsx
+++ b/src/test/resources/xls/data.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basil\Desktop\Proyectos\Java\gsmarena-automation\src\test\resources\xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80CCAE4C-496E-487B-A37B-119583E25A5C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B3A6680-5E54-4D9B-900D-62CE0297C5F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3" xr2:uid="{4B7686D2-16BC-4053-ABE4-B243528E2D9E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4B7686D2-16BC-4053-ABE4-B243528E2D9E}"/>
   </bookViews>
   <sheets>
-    <sheet name="login" sheetId="2" r:id="rId1"/>
-    <sheet name="registration" sheetId="1" r:id="rId2"/>
-    <sheet name="logout" sheetId="3" r:id="rId3"/>
-    <sheet name="search" sheetId="4" r:id="rId4"/>
+    <sheet name="loginFail" sheetId="5" r:id="rId1"/>
+    <sheet name="loginValid" sheetId="2" r:id="rId2"/>
+    <sheet name="registrationValid" sheetId="6" r:id="rId3"/>
+    <sheet name="registrationFail" sheetId="1" r:id="rId4"/>
+    <sheet name="logout" sheetId="3" r:id="rId5"/>
+    <sheet name="search" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="27">
   <si>
     <t>Execute</t>
   </si>
@@ -60,16 +62,7 @@
     <t>remo123</t>
   </si>
   <si>
-    <t>success</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
     <t>remo124remo124remo124remo124remo124remo124</t>
-  </si>
-  <si>
-    <t>false</t>
   </si>
   <si>
     <t>remoreoreoremo</t>
@@ -531,11 +524,62 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8CFC1D7-79F1-4564-B440-B946DFFFDEB3}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{6BF52AB9-F8F3-43BF-9E42-17968D128CAA}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{599B710B-7680-45F6-B8F8-7A039DCA93A3}">
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -560,46 +604,27 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>14</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2"/>
@@ -618,20 +643,78 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{6BF52AB9-F8F3-43BF-9E42-17968D128CAA}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{DD36749F-653A-443F-9A25-E464244EC3F9}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{DD36749F-653A-443F-9A25-E464244EC3F9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{584027FD-4A63-47D7-9F1D-81016CEEBCBE}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="28" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
+    <col min="5" max="5" width="34" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{AE600E01-B305-486F-9E67-DDB4EF1E3199}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC30FEF6-CA25-4072-8D5B-EC48BF940C08}">
   <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B3"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -657,53 +740,31 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>8</v>
-      </c>
+      <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>9</v>
-      </c>
+      <c r="F2" s="2"/>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
     <row r="3" spans="1:8">
-      <c r="A3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>11</v>
-      </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
@@ -744,15 +805,14 @@
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{E89ACBFA-B007-40BC-BB99-D5FE6CAD1E7E}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{D3CE954E-0FC5-468C-9C78-3B6829AF252E}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{D3CE954E-0FC5-468C-9C78-3B6829AF252E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9467650-D049-4667-BCD8-B8E066D55C0F}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -788,16 +848,16 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -808,11 +868,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FFD3F94-9E32-444E-AB07-0CBAB4C310E0}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -829,20 +889,20 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="3"/>
@@ -852,21 +912,21 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>